<commit_message>
se realizo todas las clases para esta semana
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
   <si>
     <t>Alumnos</t>
   </si>
@@ -578,7 +578,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +702,9 @@
       <c r="G3" t="s">
         <v>3</v>
       </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -725,6 +728,9 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -745,6 +751,9 @@
       <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -768,6 +777,9 @@
       <c r="G6" t="s">
         <v>3</v>
       </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -791,6 +803,9 @@
       <c r="G7" t="s">
         <v>3</v>
       </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -860,6 +875,9 @@
       <c r="G10" t="s">
         <v>3</v>
       </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -927,6 +945,9 @@
       <c r="G13" t="s">
         <v>3</v>
       </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -950,6 +971,9 @@
       <c r="G14" t="s">
         <v>3</v>
       </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -991,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18</v>
       </c>
@@ -1014,7 +1038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1036,8 +1060,11 @@
       <c r="G18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1060,7 +1087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1082,8 +1109,11 @@
       <c r="G20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1105,8 +1135,11 @@
       <c r="G21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1125,8 +1158,11 @@
       <c r="G22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1148,8 +1184,11 @@
       <c r="G23" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1172,7 +1211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1194,8 +1233,11 @@
       <c r="G25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1217,8 +1259,11 @@
       <c r="G26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -1241,7 +1286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1260,8 +1305,11 @@
       <c r="F28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1281,6 +1329,9 @@
         <v>3</v>
       </c>
       <c r="G29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se subio toda la informacion de clases para informatica basica e aplicada
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="60">
   <si>
     <t>Control Asistencias</t>
   </si>
@@ -230,12 +230,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,6 +250,12 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -301,10 +301,10 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,23 +314,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,8 +342,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -355,8 +355,8 @@
   </sheetPr>
   <dimension ref="B1:X30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -364,9 +364,8 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5748987854251"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="3"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="3.71255060728745"/>
-    <col collapsed="false" hidden="false" max="24" min="8" style="0" width="3"/>
+    <col collapsed="false" hidden="true" max="9" min="5" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="24" min="10" style="0" width="3"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
@@ -686,6 +685,9 @@
       <c r="K9" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="L9" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="n">
@@ -874,6 +876,9 @@
         <v>5</v>
       </c>
       <c r="K15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego toda la inforamcion
</commit_message>
<xml_diff>
--- a/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
+++ b/2015-2016/clases/computacion_aplicada_2/control_asistencia.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="60">
   <si>
     <t>Control Asistencias</t>
   </si>
@@ -230,6 +230,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -250,12 +256,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -301,10 +301,10 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -314,23 +314,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,8 +342,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -355,16 +355,16 @@
   </sheetPr>
   <dimension ref="B1:X30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N9" activeCellId="0" sqref="N9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5748987854251"/>
-    <col collapsed="false" hidden="true" max="11" min="4" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="24" min="12" style="0" width="3"/>
+    <col collapsed="false" hidden="true" max="13" min="4" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="24" min="14" style="0" width="3"/>
     <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
@@ -498,6 +498,12 @@
       <c r="N3" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="n">
@@ -539,6 +545,12 @@
       <c r="N4" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="n">
@@ -571,6 +583,12 @@
       <c r="N5" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="n">
@@ -612,6 +630,12 @@
       <c r="N6" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="n">
@@ -648,6 +672,12 @@
         <v>5</v>
       </c>
       <c r="N7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -688,8 +718,14 @@
       <c r="N8" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="n">
         <v>7</v>
       </c>
@@ -724,6 +760,12 @@
         <v>5</v>
       </c>
       <c r="N9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="0" t="s">
         <v>5</v>
       </c>
     </row>
@@ -767,6 +809,12 @@
       <c r="N10" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="n">
@@ -805,6 +853,12 @@
       <c r="N11" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="n">
@@ -838,6 +892,12 @@
       <c r="N12" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="n">
@@ -879,6 +939,12 @@
       <c r="N13" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="n">
@@ -920,6 +986,12 @@
       <c r="N14" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -952,6 +1024,12 @@
       <c r="N15" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
@@ -990,6 +1068,12 @@
       <c r="N16" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="n">
@@ -1028,6 +1112,12 @@
       <c r="N17" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="n">
@@ -1069,6 +1159,12 @@
       <c r="N18" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="n">
@@ -1107,6 +1203,12 @@
       <c r="N19" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="n">
@@ -1148,6 +1250,12 @@
       <c r="N20" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O20" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="n">
@@ -1189,6 +1297,12 @@
       <c r="N21" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O21" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="n">
@@ -1224,6 +1338,12 @@
       <c r="N22" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="n">
@@ -1265,6 +1385,12 @@
       <c r="N23" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="n">
@@ -1306,6 +1432,12 @@
       <c r="N24" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="n">
@@ -1347,6 +1479,12 @@
       <c r="N25" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="n">
@@ -1388,6 +1526,12 @@
       <c r="N26" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O26" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="n">
@@ -1426,6 +1570,12 @@
       <c r="N27" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="n">
@@ -1464,6 +1614,12 @@
       <c r="N28" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="n">
@@ -1505,6 +1661,12 @@
       <c r="N29" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="O29" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P29" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="n">
@@ -1544,6 +1706,12 @@
         <v>5</v>
       </c>
       <c r="N30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" s="0" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>